<commit_message>
final key timing for barbosa
</commit_message>
<xml_diff>
--- a/KeyTiming.xlsx
+++ b/KeyTiming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bfuller/Research/fhipe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96B668B-8AB7-2542-A15A-0AD31D19BA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386DF3FB-5648-3641-A8FE-D36371B9A6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="500" windowWidth="22400" windowHeight="27720" xr2:uid="{37823D2C-F5F5-0B45-B928-652F02E86849}"/>
   </bookViews>
@@ -255,10 +255,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -327,16 +327,19 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$24</c:f>
+              <c:f>Sheet1!$B$2:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
@@ -405,6 +408,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>14938</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16711</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -736,10 +742,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -808,16 +814,19 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$24</c:f>
+              <c:f>Sheet1!$C$2:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>12182</c:v>
                 </c:pt>
@@ -886,6 +895,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>5173148</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5630670</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2239,13 +2251,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>161471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>59871</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2573,7 +2585,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2844,63 +2856,71 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>512</v>
+        <v>240</v>
       </c>
       <c r="B25">
-        <f>A25*A25*A25*0.0019/86400</f>
-        <v>2.9515472592592591</v>
+        <v>16711</v>
       </c>
       <c r="C25">
-        <f>A25*A25*96.95</f>
-        <v>25414860.800000001</v>
-      </c>
-      <c r="D25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" t="s">
-        <v>5</v>
+        <v>5630670</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1024</v>
+        <v>512</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:B27" si="0">A26*A26*A26*0.0019/86400</f>
-        <v>23.612378074074073</v>
+        <f>A26*A26*A26*0.0019/86400</f>
+        <v>2.9515472592592591</v>
       </c>
       <c r="C26">
         <f>A26*A26*96.95</f>
-        <v>101659443.2</v>
+        <v>25414860.800000001</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>4096</v>
+        <v>1024</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
-        <v>1511.1921967407407</v>
+        <f t="shared" ref="B27:B28" si="0">A27*A27*A27*0.0019/86400</f>
+        <v>23.612378074074073</v>
+      </c>
+      <c r="C27">
+        <f>A27*A27*96.95</f>
+        <v>101659443.2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f>A27*8</f>
-        <v>32768</v>
+        <v>4096</v>
       </c>
       <c r="B28">
-        <f>A28*A28*A28*0.0019/86400</f>
-        <v>773730.40473125922</v>
+        <f t="shared" si="0"/>
+        <v>1511.1921967407407</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
+      <c r="A29">
+        <f>A28*8</f>
+        <v>32768</v>
+      </c>
+      <c r="B29">
+        <f>A29*A29*A29*0.0019/86400</f>
+        <v>773730.40473125922</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>

</xml_diff>